<commit_message>
Fixed token creation script. Added charts. Fixed student table display filter. Added dummy data.
</commit_message>
<xml_diff>
--- a/src/templates/sf9.xlsx
+++ b/src/templates/sf9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\acemnhs_gs\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA494D9B-B949-4993-87BF-3212565E2ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F634E49-D839-4BE6-9EB8-0E5A9C3434B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT" sheetId="149" r:id="rId1"/>
@@ -861,9 +861,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -873,7 +870,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
@@ -2268,7 +2268,7 @@
       <c r="K13" s="67"/>
       <c r="L13" s="67"/>
       <c r="M13" s="67"/>
-      <c r="W13" s="39"/>
+      <c r="W13" s="38"/>
     </row>
     <row r="14" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="25"/>
@@ -2392,7 +2392,7 @@
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
       <c r="U23" s="15"/>
-      <c r="Y23" s="37"/>
+      <c r="Y23" s="36"/>
     </row>
     <row r="24" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="8" t="s">
@@ -2950,7 +2950,7 @@
   <dimension ref="A3:AB29"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" zoomScale="124" zoomScaleNormal="124" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="16.3" x14ac:dyDescent="0.6"/>
@@ -3175,8 +3175,10 @@
       <c r="Q7" s="26">
         <v>90</v>
       </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
+      <c r="R7" s="26">
+        <v>90</v>
+      </c>
+      <c r="S7" s="37"/>
       <c r="T7" s="23"/>
       <c r="U7" s="75" t="s">
         <v>118</v>
@@ -3241,7 +3243,9 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="R8" s="26">
+        <v>90</v>
+      </c>
       <c r="S8" s="26"/>
       <c r="T8" s="23"/>
       <c r="U8" s="76"/>
@@ -3303,7 +3307,9 @@
       <c r="O9" s="112"/>
       <c r="P9" s="112"/>
       <c r="Q9" s="112"/>
-      <c r="R9" s="112"/>
+      <c r="R9" s="112">
+        <v>90</v>
+      </c>
       <c r="S9" s="112"/>
       <c r="T9" s="23"/>
       <c r="U9" s="76"/>
@@ -3397,7 +3403,9 @@
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
+      <c r="R11" s="26">
+        <v>90</v>
+      </c>
       <c r="S11" s="26"/>
       <c r="T11" s="23"/>
       <c r="U11" s="76"/>
@@ -3459,7 +3467,9 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
+      <c r="R12" s="26">
+        <v>90</v>
+      </c>
       <c r="S12" s="26"/>
       <c r="T12" s="23"/>
       <c r="U12" s="77"/>
@@ -3521,7 +3531,9 @@
       <c r="O13" s="133"/>
       <c r="P13" s="133"/>
       <c r="Q13" s="133"/>
-      <c r="R13" s="133"/>
+      <c r="R13" s="112">
+        <v>90</v>
+      </c>
       <c r="S13" s="112"/>
       <c r="U13" s="75" t="s">
         <v>57</v>
@@ -3554,7 +3566,7 @@
       <c r="O14" s="133"/>
       <c r="P14" s="133"/>
       <c r="Q14" s="133"/>
-      <c r="R14" s="133"/>
+      <c r="R14" s="113"/>
       <c r="S14" s="113"/>
       <c r="U14" s="135"/>
       <c r="V14" s="141"/>
@@ -3615,7 +3627,9 @@
       <c r="O15" s="133"/>
       <c r="P15" s="133"/>
       <c r="Q15" s="133"/>
-      <c r="R15" s="133"/>
+      <c r="R15" s="112">
+        <v>90</v>
+      </c>
       <c r="S15" s="112"/>
       <c r="U15" s="135"/>
       <c r="V15" s="144"/>
@@ -3644,7 +3658,7 @@
       <c r="O16" s="133"/>
       <c r="P16" s="133"/>
       <c r="Q16" s="133"/>
-      <c r="R16" s="133"/>
+      <c r="R16" s="113"/>
       <c r="S16" s="113"/>
       <c r="U16" s="135"/>
       <c r="V16" s="114" t="s">
@@ -3703,12 +3717,30 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
+      <c r="N17" s="26">
+        <f>SUM(N18:N21)/4</f>
+        <v>77.5</v>
+      </c>
+      <c r="O17" s="26">
+        <f t="shared" ref="O17:Q17" si="0">SUM(O18:O21)/4</f>
+        <v>77.5</v>
+      </c>
+      <c r="P17" s="26">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="Q17" s="26">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="R17" s="37">
+        <f>SUM(N17:Q17)/4</f>
+        <v>77.5</v>
+      </c>
+      <c r="S17" s="37" t="str">
+        <f>IF(R17&gt;=74, "PASSED", "FAILED")</f>
+        <v>PASSED</v>
+      </c>
       <c r="U17" s="136"/>
       <c r="V17" s="120"/>
       <c r="W17" s="121"/>
@@ -3764,12 +3796,26 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="40"/>
+      <c r="N18" s="26">
+        <v>75</v>
+      </c>
+      <c r="O18" s="26">
+        <v>75</v>
+      </c>
+      <c r="P18" s="26">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>75</v>
+      </c>
+      <c r="R18" s="37">
+        <f t="shared" ref="R18:R21" si="1">SUM(N18:Q18)/4</f>
+        <v>75</v>
+      </c>
+      <c r="S18" s="37" t="str">
+        <f t="shared" ref="S18:S21" si="2">IF(R18&gt;75, "FAILED", "PASSED")</f>
+        <v>PASSED</v>
+      </c>
       <c r="U18" s="75" t="s">
         <v>61</v>
       </c>
@@ -3829,12 +3875,26 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
+      <c r="N19" s="26">
+        <v>85</v>
+      </c>
+      <c r="O19" s="26">
+        <v>85</v>
+      </c>
+      <c r="P19" s="26">
+        <v>85</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>85</v>
+      </c>
+      <c r="R19" s="37">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="S19" s="37" t="str">
+        <f t="shared" si="2"/>
+        <v>FAILED</v>
+      </c>
       <c r="U19" s="136"/>
       <c r="V19" s="120"/>
       <c r="W19" s="121"/>
@@ -3890,12 +3950,26 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
+      <c r="N20" s="26">
+        <v>75</v>
+      </c>
+      <c r="O20" s="26">
+        <v>75</v>
+      </c>
+      <c r="P20" s="26">
+        <v>75</v>
+      </c>
+      <c r="Q20" s="26">
+        <v>75</v>
+      </c>
+      <c r="R20" s="37">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="S20" s="37" t="str">
+        <f t="shared" si="2"/>
+        <v>PASSED</v>
+      </c>
       <c r="U20" s="75" t="s">
         <v>63</v>
       </c>
@@ -3955,12 +4029,26 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
+      <c r="N21" s="26">
+        <v>75</v>
+      </c>
+      <c r="O21" s="26">
+        <v>75</v>
+      </c>
+      <c r="P21" s="26">
+        <v>75</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>75</v>
+      </c>
+      <c r="R21" s="37">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="S21" s="37" t="str">
+        <f t="shared" si="2"/>
+        <v>PASSED</v>
+      </c>
       <c r="U21" s="135"/>
       <c r="V21" s="120"/>
       <c r="W21" s="121"/>
@@ -3981,7 +4069,14 @@
       <c r="O22" s="151"/>
       <c r="P22" s="151"/>
       <c r="Q22" s="152"/>
-      <c r="R22" s="36"/>
+      <c r="R22" s="39">
+        <f>(R7+R8+R9+R11+R12+R13+R15)/7</f>
+        <v>90</v>
+      </c>
+      <c r="S22" s="40" t="str">
+        <f>IF(R22&gt;=74, "PASSED", "FAILED")</f>
+        <v>PASSED</v>
+      </c>
       <c r="U22" s="135"/>
       <c r="V22" s="114" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Updated templates. Updated SQL file.
</commit_message>
<xml_diff>
--- a/src/templates/sf9.xlsx
+++ b/src/templates/sf9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\acemnhs_gs\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294A7697-CC93-41CA-9779-2CBB0E829B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5382FFAB-AA84-4143-B3B0-B03290D825B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT" sheetId="149" r:id="rId1"/>
@@ -24,6 +24,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -564,12 +575,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -754,7 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -863,6 +880,72 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
@@ -871,6 +954,30 @@
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -880,134 +987,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1021,6 +1106,96 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1044,10 +1219,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1056,159 +1227,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1971,295 +1991,295 @@
       <selection activeCell="P33" sqref="P33:T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="14" width="3.88671875" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.3046875" customWidth="1"/>
+    <col min="2" max="14" width="3.84375" customWidth="1"/>
+    <col min="15" max="15" width="10.69140625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="10.88671875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="4.5546875" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" customWidth="1"/>
-    <col min="28" max="28" width="7.33203125" customWidth="1"/>
-    <col min="29" max="29" width="12.109375" customWidth="1"/>
+    <col min="24" max="24" width="10.84375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="12.3046875" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="4.53515625" customWidth="1"/>
+    <col min="27" max="27" width="9.07421875" customWidth="1"/>
+    <col min="28" max="28" width="7.3046875" customWidth="1"/>
+    <col min="29" max="29" width="12.07421875" customWidth="1"/>
     <col min="30" max="30" width="10" customWidth="1"/>
     <col min="31" max="31" width="7" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" customWidth="1"/>
+    <col min="32" max="32" width="9.3046875" customWidth="1"/>
     <col min="33" max="33" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="44"/>
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A4" s="72"/>
+      <c r="B4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="Q4" s="49" t="s">
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="Q4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-    </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="45"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="Q5" s="49" t="s">
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A5" s="73"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="Q5" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-    </row>
-    <row r="6" spans="1:23" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="Q6" s="50" t="s">
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+    </row>
+    <row r="6" spans="1:23" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="73"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="Q6" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="50"/>
-    </row>
-    <row r="7" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A7" s="51" t="s">
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+    </row>
+    <row r="7" spans="1:23" ht="17.600000000000001" x14ac:dyDescent="0.65">
+      <c r="A7" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="49" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-    </row>
-    <row r="8" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="55" t="s">
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+    </row>
+    <row r="8" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="64"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-    </row>
-    <row r="9" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+    </row>
+    <row r="9" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="60"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="57"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="66" t="s">
+      <c r="Q10" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
-    </row>
-    <row r="11" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="Q11" s="55" t="s">
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+    </row>
+    <row r="11" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="53"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="Q11" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
-    </row>
-    <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="59" t="s">
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+    </row>
+    <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="65" t="s">
+      <c r="Q12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="61"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="53"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
       <c r="W13" s="38"/>
     </row>
-    <row r="14" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="25"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2274,39 +2294,39 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="68" t="s">
+    <row r="16" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-    </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P17" s="69" t="s">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+    </row>
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P17" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-    </row>
-    <row r="18" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+    </row>
+    <row r="18" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
@@ -2322,7 +2342,7 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B19" s="8"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
@@ -2330,7 +2350,7 @@
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
@@ -2346,7 +2366,7 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B21" s="8"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
@@ -2354,7 +2374,7 @@
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="8" t="s">
         <v>27</v>
       </c>
@@ -2373,7 +2393,7 @@
       <c r="T22" s="12"/>
       <c r="U22" s="13"/>
     </row>
-    <row r="23" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B23" s="8"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -2383,7 +2403,7 @@
       <c r="U23" s="15"/>
       <c r="Y23" s="36"/>
     </row>
-    <row r="24" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="8" t="s">
         <v>28</v>
       </c>
@@ -2409,7 +2429,7 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B25" s="8"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -2425,21 +2445,21 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="B26" s="70" t="s">
+    <row r="26" spans="1:25" ht="17.149999999999999" x14ac:dyDescent="0.6">
+      <c r="B26" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
       <c r="P26" s="14" t="s">
         <v>100</v>
       </c>
@@ -2456,19 +2476,19 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="71"/>
-      <c r="M27" s="71"/>
+    <row r="27" spans="1:25" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
@@ -2483,7 +2503,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="34" t="s">
         <v>102</v>
       </c>
@@ -2515,7 +2535,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:25" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="34" t="s">
         <v>105</v>
       </c>
@@ -2547,7 +2567,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2579,7 +2599,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:25" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2604,7 +2624,7 @@
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
     </row>
-    <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="1" t="s">
         <v>109</v>
       </c>
@@ -2633,23 +2653,23 @@
       <c r="T32" s="15"/>
       <c r="U32" s="15"/>
     </row>
-    <row r="33" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A33" s="1"/>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="49" t="s">
+      <c r="J33" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2662,36 +2682,36 @@
       <c r="T33" s="15"/>
       <c r="U33" s="15"/>
     </row>
-    <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
+    <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="72" t="s">
+      <c r="H34" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
       <c r="O34" s="8"/>
-      <c r="P34" s="73" t="s">
+      <c r="P34" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="Q34" s="73"/>
+      <c r="Q34" s="44"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
     </row>
-    <row r="35" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.65">
       <c r="P35" s="20" t="s">
         <v>35</v>
       </c>
@@ -2701,21 +2721,21 @@
       <c r="T35" s="15"/>
       <c r="U35" s="15"/>
     </row>
-    <row r="36" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="68"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="68"/>
-      <c r="N36" s="68"/>
+    <row r="36" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
       <c r="P36" s="12" t="s">
         <v>36</v>
       </c>
@@ -2725,23 +2745,23 @@
       <c r="T36" s="14"/>
       <c r="U36" s="15"/>
     </row>
-    <row r="37" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="70" t="s">
+    <row r="37" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A37" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
       <c r="P37" s="14" t="s">
         <v>38</v>
       </c>
@@ -2751,7 +2771,7 @@
       <c r="T37" s="15"/>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="P38" s="14" t="s">
         <v>39</v>
       </c>
@@ -2761,7 +2781,7 @@
       <c r="T38" s="15"/>
       <c r="U38" s="15"/>
     </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A39" s="35" t="s">
         <v>111</v>
       </c>
@@ -2785,7 +2805,7 @@
       <c r="T39" s="15"/>
       <c r="U39" s="15"/>
     </row>
-    <row r="40" spans="1:21" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="34" t="s">
         <v>112</v>
       </c>
@@ -2804,18 +2824,18 @@
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
-      <c r="P40" s="68" t="s">
+      <c r="P40" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="Q40" s="68"/>
-      <c r="R40" s="68"/>
-      <c r="S40" s="68" t="s">
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="T40" s="68"/>
-      <c r="U40" s="68"/>
-    </row>
-    <row r="41" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
+    </row>
+    <row r="41" spans="1:21" ht="17.600000000000001" x14ac:dyDescent="0.65">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
@@ -2832,40 +2852,63 @@
       <c r="L41" s="21"/>
       <c r="M41" s="21"/>
       <c r="N41" s="21"/>
-      <c r="P41" s="70" t="s">
+      <c r="P41" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="Q41" s="70"/>
-      <c r="R41" s="70"/>
-      <c r="S41" s="70" t="s">
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="T41" s="70"/>
-      <c r="U41" s="70"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="42"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="79">
-    <mergeCell ref="S40:U40"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="S41:U41"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="A36:N36"/>
-    <mergeCell ref="A37:N37"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="P17:U17"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N8"/>
+    <mergeCell ref="O4:O8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="Q8:T9"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="Q12:T12"/>
     <mergeCell ref="Q10:T10"/>
     <mergeCell ref="Q11:T11"/>
@@ -2882,49 +2925,26 @@
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="L9:L11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="Q7:T7"/>
-    <mergeCell ref="Q8:T9"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N8"/>
-    <mergeCell ref="O4:O8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="S40:U40"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="S41:U41"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="A36:N36"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="P40:R40"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
@@ -2938,74 +2958,74 @@
   <sheetPr codeName="Sheet127"/>
   <dimension ref="A3:AB29"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="124" zoomScaleNormal="124" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" zoomScale="124" zoomScaleNormal="124" zoomScaleSheetLayoutView="124" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10:Z12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="16.3" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="2" max="2" width="9.07421875" style="1"/>
     <col min="3" max="3" width="4" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="13" width="10.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="4.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.84375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="13" width="10.84375" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="4.84375" style="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.5546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.3046875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.69140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.53515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="7.53515625" style="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="1" customWidth="1"/>
     <col min="24" max="24" width="6" style="1" customWidth="1"/>
-    <col min="25" max="28" width="5.6640625" style="1" customWidth="1"/>
-    <col min="29" max="35" width="9.109375" style="1"/>
-    <col min="36" max="36" width="9.109375" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.109375" style="1"/>
+    <col min="25" max="28" width="5.69140625" style="1" customWidth="1"/>
+    <col min="29" max="35" width="9.07421875" style="1"/>
+    <col min="36" max="36" width="9.07421875" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.07421875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:28" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="70" t="s">
+    <row r="3" spans="1:28" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A3" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
       <c r="T3" s="14"/>
-      <c r="U3" s="70" t="s">
+      <c r="U3" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-    </row>
-    <row r="4" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="42"/>
+    </row>
+    <row r="4" spans="1:28" ht="17.600000000000001" x14ac:dyDescent="0.65">
       <c r="S4" s="20"/>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="142"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
@@ -3016,37 +3036,37 @@
       <c r="K5" s="32"/>
       <c r="L5" s="32"/>
       <c r="M5" s="32"/>
-      <c r="N5" s="91" t="s">
+      <c r="N5" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="93" t="s">
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="145" t="s">
         <v>46</v>
       </c>
-      <c r="S5" s="95" t="s">
+      <c r="S5" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="97" t="s">
+      <c r="U5" s="149" t="s">
         <v>47</v>
       </c>
-      <c r="V5" s="91" t="s">
+      <c r="V5" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="W5" s="91"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91" t="s">
+      <c r="W5" s="143"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-    </row>
-    <row r="6" spans="1:28" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
+      <c r="Z5" s="143"/>
+      <c r="AA5" s="143"/>
+      <c r="AB5" s="143"/>
+    </row>
+    <row r="6" spans="1:28" ht="20.6" x14ac:dyDescent="0.75">
+      <c r="A6" s="142"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="142"/>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
         <v>119</v>
@@ -3087,12 +3107,12 @@
       <c r="Q6" s="22">
         <v>4</v>
       </c>
-      <c r="R6" s="94"/>
-      <c r="S6" s="96"/>
-      <c r="U6" s="97"/>
-      <c r="V6" s="91"/>
-      <c r="W6" s="91"/>
-      <c r="X6" s="91"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="148"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="143"/>
+      <c r="X6" s="143"/>
       <c r="Y6" s="24">
         <v>1</v>
       </c>
@@ -3106,12 +3126,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="74" t="s">
+    <row r="7" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="31" t="e">
         <f>IF(#REF!="GRADE-7","FILIPINO7",IF(#REF!="GRADE-8","FILIPINO8",IF(#REF!="GRADE-9","FILIPINO9",IF(#REF!="GRADE-10","FILIPINO10",""))))</f>
         <v>#REF!</v>
@@ -3169,25 +3189,25 @@
       </c>
       <c r="S7" s="37"/>
       <c r="T7" s="23"/>
-      <c r="U7" s="75" t="s">
+      <c r="U7" s="90" t="s">
         <v>118</v>
       </c>
-      <c r="V7" s="78" t="s">
+      <c r="V7" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="W7" s="79"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="87"/>
-      <c r="Z7" s="87"/>
-      <c r="AA7" s="87"/>
-      <c r="AB7" s="87"/>
-    </row>
-    <row r="8" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="99" t="s">
+      <c r="W7" s="134"/>
+      <c r="X7" s="135"/>
+      <c r="Y7" s="109"/>
+      <c r="Z7" s="109"/>
+      <c r="AA7" s="109"/>
+      <c r="AB7" s="109"/>
+    </row>
+    <row r="8" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A8" s="150" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="150"/>
       <c r="D8" s="31" t="e">
         <f>IF(#REF!="GRADE-7","ENGLISH7",IF(#REF!="GRADE-8","ENGLISH8",IF(#REF!="GRADE-9","ENGLISH9",IF(#REF!="GRADE-10","ENGLISH10",""))))</f>
         <v>#REF!</v>
@@ -3237,117 +3257,117 @@
       </c>
       <c r="S8" s="26"/>
       <c r="T8" s="23"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="82"/>
-      <c r="X8" s="83"/>
-      <c r="Y8" s="88"/>
-      <c r="Z8" s="88"/>
-      <c r="AA8" s="88"/>
-      <c r="AB8" s="88"/>
-    </row>
-    <row r="9" spans="1:28" ht="8.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="106" t="s">
+      <c r="U8" s="131"/>
+      <c r="V8" s="136"/>
+      <c r="W8" s="137"/>
+      <c r="X8" s="138"/>
+      <c r="Y8" s="110"/>
+      <c r="Z8" s="110"/>
+      <c r="AA8" s="110"/>
+      <c r="AB8" s="110"/>
+    </row>
+    <row r="9" spans="1:28" ht="8.25" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="100" t="e">
+      <c r="B9" s="125"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="151" t="e">
         <f>IF(#REF!="GRADE-7","MATHEMATICS7",IF(#REF!="GRADE-8","MATHEMATICS8",IF(#REF!="GRADE-9","MATHEMATICS9",IF(#REF!="GRADE-10","MATHEMATICS10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" s="104" t="e">
+      <c r="E9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="82" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M9" s="104" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N9" s="112"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="112">
+      <c r="K9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M9" s="82" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87">
         <v>90</v>
       </c>
-      <c r="S9" s="112"/>
+      <c r="S9" s="87"/>
       <c r="T9" s="23"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="84"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="89"/>
-      <c r="Z9" s="89"/>
-      <c r="AA9" s="89"/>
-      <c r="AB9" s="89"/>
-    </row>
-    <row r="10" spans="1:28" ht="6.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="109"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="105"/>
-      <c r="N10" s="113"/>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="113"/>
-      <c r="R10" s="113"/>
-      <c r="S10" s="113"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="140"/>
+      <c r="X9" s="141"/>
+      <c r="Y9" s="111"/>
+      <c r="Z9" s="111"/>
+      <c r="AA9" s="111"/>
+      <c r="AB9" s="111"/>
+    </row>
+    <row r="10" spans="1:28" ht="6.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="127"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="88"/>
+      <c r="S10" s="88"/>
       <c r="T10" s="23"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="114" t="s">
+      <c r="U10" s="131"/>
+      <c r="V10" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="W10" s="115"/>
-      <c r="X10" s="116"/>
-      <c r="Y10" s="98"/>
-      <c r="Z10" s="98"/>
-      <c r="AA10" s="98"/>
-      <c r="AB10" s="98"/>
-    </row>
-    <row r="11" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="99" t="s">
+      <c r="W10" s="94"/>
+      <c r="X10" s="95"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+      <c r="AB10" s="89"/>
+    </row>
+    <row r="11" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A11" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="31" t="e">
         <f>IF(#REF!="GRADE-7","SCIENCE7",IF(#REF!="GRADE-8","SCIENCE8",IF(#REF!="GRADE-9","SCIENCE9",IF(#REF!="GRADE-10","SCIENCE10",""))))</f>
         <v>#REF!</v>
@@ -3397,21 +3417,21 @@
       </c>
       <c r="S11" s="26"/>
       <c r="T11" s="23"/>
-      <c r="U11" s="76"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="118"/>
-      <c r="X11" s="119"/>
-      <c r="Y11" s="98"/>
-      <c r="Z11" s="98"/>
-      <c r="AA11" s="98"/>
-      <c r="AB11" s="98"/>
-    </row>
-    <row r="12" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="99" t="s">
+      <c r="U11" s="131"/>
+      <c r="V11" s="112"/>
+      <c r="W11" s="113"/>
+      <c r="X11" s="114"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+      <c r="AB11" s="89"/>
+    </row>
+    <row r="12" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A12" s="150" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="150"/>
       <c r="D12" s="31" t="e">
         <f>IF(#REF!="GRADE-7","AP7",IF(#REF!="GRADE-8","AP8",IF(#REF!="GRADE-9","AP9",IF(#REF!="GRADE-10","AP10",""))))</f>
         <v>#REF!</v>
@@ -3461,211 +3481,211 @@
       </c>
       <c r="S12" s="26"/>
       <c r="T12" s="23"/>
-      <c r="U12" s="77"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="121"/>
-      <c r="X12" s="122"/>
-      <c r="Y12" s="98"/>
-      <c r="Z12" s="98"/>
-      <c r="AA12" s="98"/>
-      <c r="AB12" s="98"/>
-    </row>
-    <row r="13" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="132" t="s">
+      <c r="U12" s="132"/>
+      <c r="V12" s="96"/>
+      <c r="W12" s="97"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+    </row>
+    <row r="13" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="132"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="102" t="e">
+      <c r="B13" s="120"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="122" t="e">
         <f>IF(#REF!="GRADE-7","ESP7",IF(#REF!="GRADE-8","ESP8",IF(#REF!="GRADE-9","ESP9",IF(#REF!="GRADE-10","ESP10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="128" t="e">
+      <c r="E13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="84" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="128" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N13" s="133"/>
-      <c r="O13" s="133"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="133"/>
-      <c r="R13" s="112">
+      <c r="K13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M13" s="84" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="87">
         <v>90</v>
       </c>
-      <c r="S13" s="112"/>
-      <c r="U13" s="75" t="s">
+      <c r="S13" s="87"/>
+      <c r="U13" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="V13" s="138" t="s">
+      <c r="V13" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="139"/>
-      <c r="X13" s="140"/>
-      <c r="Y13" s="87"/>
-      <c r="Z13" s="87"/>
-      <c r="AA13" s="87"/>
-      <c r="AB13" s="87"/>
-    </row>
-    <row r="14" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="132"/>
-      <c r="B14" s="132"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
-      <c r="G14" s="129"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="129"/>
-      <c r="K14" s="129"/>
-      <c r="L14" s="129"/>
-      <c r="M14" s="129"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
-      <c r="U14" s="135"/>
-      <c r="V14" s="141"/>
-      <c r="W14" s="142"/>
-      <c r="X14" s="143"/>
-      <c r="Y14" s="88"/>
-      <c r="Z14" s="88"/>
-      <c r="AA14" s="88"/>
-      <c r="AB14" s="88"/>
-    </row>
-    <row r="15" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="134" t="s">
+      <c r="W13" s="101"/>
+      <c r="X13" s="102"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
+      <c r="AB13" s="109"/>
+    </row>
+    <row r="14" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="120"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="88"/>
+      <c r="U14" s="91"/>
+      <c r="V14" s="103"/>
+      <c r="W14" s="104"/>
+      <c r="X14" s="105"/>
+      <c r="Y14" s="110"/>
+      <c r="Z14" s="110"/>
+      <c r="AA14" s="110"/>
+      <c r="AB14" s="110"/>
+    </row>
+    <row r="15" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="126" t="e">
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="118" t="e">
         <f>IF(#REF!="GRADE-7","TLE7",IF(#REF!="GRADE-8","TLE8",IF(#REF!="GRADE-9","TLE9",IF(#REF!="GRADE-10","TLE10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="130" t="e">
+      <c r="E15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J15" s="74" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M15" s="130" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N15" s="133"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="133"/>
-      <c r="Q15" s="133"/>
-      <c r="R15" s="112">
+      <c r="K15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M15" s="74" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="87">
         <v>90</v>
       </c>
-      <c r="S15" s="112"/>
-      <c r="U15" s="135"/>
-      <c r="V15" s="144"/>
-      <c r="W15" s="145"/>
-      <c r="X15" s="146"/>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="89"/>
-      <c r="AA15" s="89"/>
-      <c r="AB15" s="89"/>
-    </row>
-    <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="134"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="133"/>
-      <c r="O16" s="133"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="133"/>
-      <c r="R16" s="113"/>
-      <c r="S16" s="113"/>
-      <c r="U16" s="135"/>
-      <c r="V16" s="114" t="s">
+      <c r="S15" s="87"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="106"/>
+      <c r="W15" s="107"/>
+      <c r="X15" s="108"/>
+      <c r="Y15" s="111"/>
+      <c r="Z15" s="111"/>
+      <c r="AA15" s="111"/>
+      <c r="AB15" s="111"/>
+    </row>
+    <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="121"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="86"/>
+      <c r="R16" s="88"/>
+      <c r="S16" s="88"/>
+      <c r="U16" s="91"/>
+      <c r="V16" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="W16" s="115"/>
-      <c r="X16" s="116"/>
-      <c r="Y16" s="98"/>
-      <c r="Z16" s="98"/>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98"/>
-    </row>
-    <row r="17" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="123" t="s">
+      <c r="W16" s="94"/>
+      <c r="X16" s="95"/>
+      <c r="Y16" s="89"/>
+      <c r="Z16" s="89"/>
+      <c r="AA16" s="89"/>
+      <c r="AB16" s="89"/>
+    </row>
+    <row r="17" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="125"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="117"/>
       <c r="D17" s="30" t="e">
         <f>IF(#REF!="GRADE-7","MAPEH7",IF(#REF!="GRADE-8","MAPEH8",IF(#REF!="GRADE-9","MAPEH9",IF(#REF!="GRADE-10","MAPEH10",""))))</f>
         <v>#REF!</v>
@@ -3730,21 +3750,21 @@
         <f>IF(R17&gt;=74, "PASSED", "FAILED")</f>
         <v>FAILED</v>
       </c>
-      <c r="U17" s="136"/>
-      <c r="V17" s="120"/>
-      <c r="W17" s="121"/>
-      <c r="X17" s="122"/>
-      <c r="Y17" s="98"/>
-      <c r="Z17" s="98"/>
-      <c r="AA17" s="98"/>
-      <c r="AB17" s="98"/>
-    </row>
-    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="U17" s="92"/>
+      <c r="V17" s="96"/>
+      <c r="W17" s="97"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="89"/>
+      <c r="AB17" s="89"/>
+    </row>
+    <row r="18" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="27"/>
-      <c r="B18" s="147" t="s">
+      <c r="B18" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="148"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="29" t="e">
         <f>IF(#REF!="GRADE-7","MUSIC7",IF(#REF!="GRADE-8","MUSIC8",IF(#REF!="GRADE-9","MUSIC9",IF(#REF!="GRADE-10","MUSIC10",""))))</f>
         <v>#REF!</v>
@@ -3789,30 +3809,30 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37" t="str">
+      <c r="R18" s="153"/>
+      <c r="S18" s="153" t="str">
         <f t="shared" ref="S18:S21" si="1">IF(R18&gt;75, "FAILED", "PASSED")</f>
         <v>PASSED</v>
       </c>
-      <c r="U18" s="75" t="s">
+      <c r="U18" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="V18" s="114" t="s">
+      <c r="V18" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="W18" s="115"/>
-      <c r="X18" s="116"/>
-      <c r="Y18" s="98"/>
-      <c r="Z18" s="98"/>
-      <c r="AA18" s="98"/>
-      <c r="AB18" s="98"/>
-    </row>
-    <row r="19" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W18" s="94"/>
+      <c r="X18" s="95"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="89"/>
+      <c r="AB18" s="89"/>
+    </row>
+    <row r="19" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="27"/>
-      <c r="B19" s="147" t="s">
+      <c r="B19" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="148"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="29" t="e">
         <f>IF(#REF!="GRADE-7","ARTS7",IF(#REF!="GRADE-8","ARTS8",IF(#REF!="GRADE-9","ARTS9",IF(#REF!="GRADE-10","ARTS10",""))))</f>
         <v>#REF!</v>
@@ -3857,26 +3877,26 @@
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37" t="str">
+      <c r="R19" s="153"/>
+      <c r="S19" s="153" t="str">
         <f t="shared" si="1"/>
         <v>PASSED</v>
       </c>
-      <c r="U19" s="136"/>
-      <c r="V19" s="120"/>
-      <c r="W19" s="121"/>
-      <c r="X19" s="122"/>
-      <c r="Y19" s="98"/>
-      <c r="Z19" s="98"/>
-      <c r="AA19" s="98"/>
-      <c r="AB19" s="98"/>
-    </row>
-    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="U19" s="92"/>
+      <c r="V19" s="96"/>
+      <c r="W19" s="97"/>
+      <c r="X19" s="98"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="89"/>
+      <c r="AB19" s="89"/>
+    </row>
+    <row r="20" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="28"/>
-      <c r="B20" s="149" t="s">
+      <c r="B20" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="150"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="33" t="e">
         <f>IF(#REF!="GRADE-7","PE7",IF(#REF!="GRADE-8","PE8",IF(#REF!="GRADE-9","PE9",IF(#REF!="GRADE-10","PE10",""))))</f>
         <v>#REF!</v>
@@ -3921,30 +3941,30 @@
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37" t="str">
+      <c r="R20" s="153"/>
+      <c r="S20" s="153" t="str">
         <f t="shared" si="1"/>
         <v>PASSED</v>
       </c>
-      <c r="U20" s="75" t="s">
+      <c r="U20" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="V20" s="114" t="s">
+      <c r="V20" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="W20" s="115"/>
-      <c r="X20" s="116"/>
-      <c r="Y20" s="98"/>
-      <c r="Z20" s="98"/>
-      <c r="AA20" s="98"/>
-      <c r="AB20" s="98"/>
-    </row>
-    <row r="21" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W20" s="94"/>
+      <c r="X20" s="95"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="89"/>
+      <c r="AB20" s="89"/>
+    </row>
+    <row r="21" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="28"/>
-      <c r="B21" s="147" t="s">
+      <c r="B21" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="148"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="29" t="e">
         <f>IF(#REF!="GRADE-7","HEALTH7",IF(#REF!="GRADE-8","HEALTH8",IF(#REF!="GRADE-9","HEALTH9",IF(#REF!="GRADE-10","HEALTH10",""))))</f>
         <v>#REF!</v>
@@ -3989,31 +4009,31 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37" t="str">
+      <c r="R21" s="153"/>
+      <c r="S21" s="153" t="str">
         <f t="shared" si="1"/>
         <v>PASSED</v>
       </c>
-      <c r="U21" s="135"/>
-      <c r="V21" s="120"/>
-      <c r="W21" s="121"/>
-      <c r="X21" s="122"/>
-      <c r="Y21" s="98"/>
-      <c r="Z21" s="98"/>
-      <c r="AA21" s="98"/>
-      <c r="AB21" s="98"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="U21" s="91"/>
+      <c r="V21" s="96"/>
+      <c r="W21" s="97"/>
+      <c r="X21" s="98"/>
+      <c r="Y21" s="89"/>
+      <c r="Z21" s="89"/>
+      <c r="AA21" s="89"/>
+      <c r="AB21" s="89"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.6">
       <c r="D22" s="1" t="e">
         <f>IF(#REF!="GRADE-7","GEN7",IF(#REF!="GRADE-8","GEN8",IF(#REF!="GRADE-9","GEN9",IF(#REF!="GRADE-10","GEN10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="N22" s="151" t="s">
+      <c r="N22" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="O22" s="151"/>
-      <c r="P22" s="151"/>
-      <c r="Q22" s="152"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="81"/>
       <c r="R22" s="39">
         <f>(R7+R8+R9+R11+R12+R13+R15)/7</f>
         <v>90</v>
@@ -4022,28 +4042,28 @@
         <f>IF(R22&gt;=74, "PASSED", "FAILED")</f>
         <v>PASSED</v>
       </c>
-      <c r="U22" s="135"/>
-      <c r="V22" s="114" t="s">
+      <c r="U22" s="91"/>
+      <c r="V22" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="W22" s="115"/>
-      <c r="X22" s="116"/>
-      <c r="Y22" s="137"/>
-      <c r="Z22" s="137"/>
-      <c r="AA22" s="137"/>
-      <c r="AB22" s="137"/>
-    </row>
-    <row r="23" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="U23" s="136"/>
-      <c r="V23" s="120"/>
-      <c r="W23" s="121"/>
-      <c r="X23" s="122"/>
-      <c r="Y23" s="137"/>
-      <c r="Z23" s="137"/>
-      <c r="AA23" s="137"/>
-      <c r="AB23" s="137"/>
-    </row>
-    <row r="24" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W22" s="94"/>
+      <c r="X22" s="95"/>
+      <c r="Y22" s="99"/>
+      <c r="Z22" s="99"/>
+      <c r="AA22" s="99"/>
+      <c r="AB22" s="99"/>
+    </row>
+    <row r="23" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="U23" s="92"/>
+      <c r="V23" s="96"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="98"/>
+      <c r="Y23" s="99"/>
+      <c r="Z23" s="99"/>
+      <c r="AA23" s="99"/>
+      <c r="AB23" s="99"/>
+    </row>
+    <row r="24" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A24" s="14" t="s">
         <v>67</v>
       </c>
@@ -4059,16 +4079,16 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="70" t="s">
+      <c r="N24" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="70" t="s">
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="S24" s="70"/>
+      <c r="S24" s="42"/>
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>
@@ -4078,7 +4098,7 @@
       <c r="Z24" s="20"/>
       <c r="AA24" s="20"/>
     </row>
-    <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A25" s="20" t="s">
         <v>69</v>
       </c>
@@ -4094,16 +4114,16 @@
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
-      <c r="N25" s="49" t="s">
+      <c r="N25" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49" t="s">
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="S25" s="49"/>
+      <c r="S25" s="47"/>
       <c r="T25" s="20"/>
       <c r="U25" s="20"/>
       <c r="V25" s="14" t="s">
@@ -4117,7 +4137,7 @@
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
     </row>
-    <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A26" s="20" t="s">
         <v>74</v>
       </c>
@@ -4133,16 +4153,16 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
-      <c r="N26" s="49" t="s">
+      <c r="N26" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49" t="s">
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="S26" s="49"/>
+      <c r="S26" s="47"/>
       <c r="T26" s="20"/>
       <c r="U26" s="20"/>
       <c r="V26" s="21" t="s">
@@ -4156,7 +4176,7 @@
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
     </row>
-    <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A27" s="20" t="s">
         <v>78</v>
       </c>
@@ -4172,16 +4192,16 @@
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
-      <c r="N27" s="49" t="s">
+      <c r="N27" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49" t="s">
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="S27" s="49"/>
+      <c r="S27" s="47"/>
       <c r="T27" s="20"/>
       <c r="U27" s="20"/>
       <c r="V27" s="21" t="s">
@@ -4195,7 +4215,7 @@
       <c r="Z27" s="20"/>
       <c r="AA27" s="20"/>
     </row>
-    <row r="28" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A28" s="20" t="s">
         <v>82</v>
       </c>
@@ -4211,16 +4231,16 @@
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
-      <c r="N28" s="49" t="s">
+      <c r="N28" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49" t="s">
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="47"/>
+      <c r="R28" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="S28" s="49"/>
+      <c r="S28" s="47"/>
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
       <c r="V28" s="21" t="s">
@@ -4234,7 +4254,7 @@
       <c r="Z28" s="20"/>
       <c r="AA28" s="20"/>
     </row>
-    <row r="29" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A29" s="20" t="s">
         <v>86</v>
       </c>
@@ -4250,16 +4270,16 @@
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
-      <c r="N29" s="49" t="s">
+      <c r="N29" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49" t="s">
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="S29" s="49"/>
+      <c r="S29" s="47"/>
       <c r="T29" s="20"/>
       <c r="U29" s="20"/>
       <c r="V29" s="21" t="s">
@@ -4275,6 +4295,103 @@
     </row>
   </sheetData>
   <mergeCells count="121">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="U7:U12"/>
+    <mergeCell ref="V7:X9"/>
+    <mergeCell ref="Y7:Y9"/>
+    <mergeCell ref="Z7:Z9"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="A5:C6"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:X6"/>
+    <mergeCell ref="Y5:AB5"/>
+    <mergeCell ref="AB10:AB12"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="AA10:AA12"/>
+    <mergeCell ref="AB7:AB9"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="Y10:Y12"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="V10:X12"/>
+    <mergeCell ref="Z13:Z15"/>
+    <mergeCell ref="AA13:AA15"/>
+    <mergeCell ref="AB13:AB15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="A13:C14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="A15:C16"/>
+    <mergeCell ref="Z18:Z19"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="AA18:AA19"/>
+    <mergeCell ref="AB18:AB19"/>
+    <mergeCell ref="U20:U23"/>
+    <mergeCell ref="V20:X21"/>
+    <mergeCell ref="Y20:Y21"/>
+    <mergeCell ref="Z20:Z21"/>
+    <mergeCell ref="AA20:AA21"/>
+    <mergeCell ref="AB20:AB21"/>
+    <mergeCell ref="V22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AB22:AB23"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="U13:U17"/>
+    <mergeCell ref="V13:X15"/>
+    <mergeCell ref="Y13:Y15"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:X19"/>
+    <mergeCell ref="Y18:Y19"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
@@ -4299,103 +4416,6 @@
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="Z18:Z19"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="AA18:AA19"/>
-    <mergeCell ref="AB18:AB19"/>
-    <mergeCell ref="U20:U23"/>
-    <mergeCell ref="V20:X21"/>
-    <mergeCell ref="Y20:Y21"/>
-    <mergeCell ref="Z20:Z21"/>
-    <mergeCell ref="AA20:AA21"/>
-    <mergeCell ref="AB20:AB21"/>
-    <mergeCell ref="V22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="AA22:AA23"/>
-    <mergeCell ref="AB22:AB23"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="U13:U17"/>
-    <mergeCell ref="V13:X15"/>
-    <mergeCell ref="Y13:Y15"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:X19"/>
-    <mergeCell ref="Y18:Y19"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="V10:X12"/>
-    <mergeCell ref="Z13:Z15"/>
-    <mergeCell ref="AA13:AA15"/>
-    <mergeCell ref="AB13:AB15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="A13:C14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="A15:C16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="U7:U12"/>
-    <mergeCell ref="V7:X9"/>
-    <mergeCell ref="Y7:Y9"/>
-    <mergeCell ref="Z7:Z9"/>
-    <mergeCell ref="AA7:AA9"/>
-    <mergeCell ref="A3:S3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="A5:C6"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:X6"/>
-    <mergeCell ref="Y5:AB5"/>
-    <mergeCell ref="AB10:AB12"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="AA10:AA12"/>
-    <mergeCell ref="AB7:AB9"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="Y10:Y12"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>